<commit_message>
1.delete unused variable 2.add default to switch function 3.add hwiocald to fix the i6l generation function 4.in order to convenient the customer's test, config the baund rate at 500K
</commit_message>
<xml_diff>
--- a/document/Design/MBs_list.xlsx
+++ b/document/Design/MBs_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="124">
   <si>
     <t>Message Buffer</t>
   </si>
@@ -377,6 +377,15 @@
   </si>
   <si>
     <t>0x1CFE8200</t>
+  </si>
+  <si>
+    <t>RXIMR</t>
+  </si>
+  <si>
+    <t>0x3FF00</t>
+  </si>
+  <si>
+    <t>0x3FFFF</t>
   </si>
 </sst>
 </file>
@@ -400,7 +409,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -408,14 +417,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,11 +750,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,9 +762,10 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -750,8 +784,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -770,33 +807,69 @@
       <c r="F2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -815,13 +888,55 @@
       <c r="F8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>123</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -840,8 +955,29 @@
       <c r="F10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -860,8 +996,29 @@
       <c r="F11" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -880,8 +1037,29 @@
       <c r="F12" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -900,8 +1078,29 @@
       <c r="F13" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>123</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -920,13 +1119,55 @@
       <c r="F14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>123</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -945,8 +1186,29 @@
       <c r="F16" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -965,8 +1227,11 @@
       <c r="F17" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -985,8 +1250,11 @@
       <c r="F18" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1005,8 +1273,11 @@
       <c r="F19" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1025,8 +1296,11 @@
       <c r="F20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1045,8 +1319,11 @@
       <c r="F21" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1065,8 +1342,11 @@
       <c r="F22" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1083,10 +1363,13 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="G23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1103,10 +1386,13 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="G24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1123,10 +1409,13 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="G25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1143,10 +1432,13 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="G26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1163,10 +1455,13 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="G27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1183,10 +1478,13 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1203,10 +1501,13 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="G29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1223,10 +1524,13 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="G30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1239,21 +1543,33 @@
       <c r="D31" t="s">
         <v>82</v>
       </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
       <c r="F31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="G31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1272,8 +1588,11 @@
       <c r="F34" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1292,8 +1611,11 @@
       <c r="F35" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1312,8 +1634,11 @@
       <c r="F36" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1332,8 +1657,11 @@
       <c r="F37" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1352,8 +1680,11 @@
       <c r="F38" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1372,8 +1703,11 @@
       <c r="F39" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1392,8 +1726,11 @@
       <c r="F40" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1412,8 +1749,11 @@
       <c r="F41" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1432,8 +1772,11 @@
       <c r="F42" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1452,8 +1795,11 @@
       <c r="F43" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1472,8 +1818,11 @@
       <c r="F44" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1492,8 +1841,11 @@
       <c r="F45" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1512,8 +1864,11 @@
       <c r="F46" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1532,8 +1887,11 @@
       <c r="F47" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1552,8 +1910,11 @@
       <c r="F48" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1572,8 +1933,11 @@
       <c r="F49" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1592,8 +1956,11 @@
       <c r="F50" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1612,8 +1979,11 @@
       <c r="F51" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1632,8 +2002,11 @@
       <c r="F52" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -1652,8 +2025,11 @@
       <c r="F53" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1672,8 +2048,11 @@
       <c r="F54" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1692,8 +2071,11 @@
       <c r="F55" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -1712,8 +2094,11 @@
       <c r="F56" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -1732,8 +2117,11 @@
       <c r="F57" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -1752,8 +2140,11 @@
       <c r="F58" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -1772,8 +2163,11 @@
       <c r="F59" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -1792,8 +2186,11 @@
       <c r="F60" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -1812,8 +2209,11 @@
       <c r="F61" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -1832,8 +2232,11 @@
       <c r="F62" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -1852,8 +2255,11 @@
       <c r="F63" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -1871,6 +2277,9 @@
       </c>
       <c r="F64" t="s">
         <v>92</v>
+      </c>
+      <c r="G64" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>